<commit_message>
add alternative analyses column for excluded studies in full text screening
</commit_message>
<xml_diff>
--- a/2. full text screening/full_text_screening.xlsx
+++ b/2. full text screening/full_text_screening.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/Research/2. Projects/1. Current (16)/Leading (7)/coexistence-microbes/2. systematic reivew/3. full text screening/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/Research/2. Projects/1. Current (12)/Leading (5)/coexistence-microbes/4. Public GitHub repo/coexistence-microbes/2. full text screening/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE786CF-D30B-0A40-A96D-2C2F57064D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B3612-DD05-C946-9BBF-CBBCBF0E9E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30320" yWindow="600" windowWidth="32340" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33940" yWindow="-1920" windowWidth="32340" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="full_text_screening" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="355">
   <si>
     <t>Authors</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>In WoS Search</t>
   </si>
   <si>
@@ -71,18 +68,6 @@
     <t>ASReview found</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>asreview</t>
-  </si>
-  <si>
-    <t>previous</t>
-  </si>
-  <si>
-    <t>discuss</t>
-  </si>
-  <si>
     <t>Hogle, SL; Hepolehto, I; Ruokolainen, L; Cairns, J; Hiltunen, T; Chase, J</t>
   </si>
   <si>
@@ -107,15 +92,6 @@
     <t>protists</t>
   </si>
   <si>
-    <t>ND-FD</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>bacteria are the resource that a ciliate population and a nematode population are competiting for. MCT is used to predict coexistence of ciliate and nematode</t>
-  </si>
-  <si>
     <t>Jackrel, SL; Schmidt, KC; Cardinale, BJ; Denef, VJ</t>
   </si>
   <si>
@@ -200,9 +176,6 @@
     <t>yeast</t>
   </si>
   <si>
-    <t>* not in Terry and Armitage as it uses invasion tests rather than "response surface" experiments to quantify coexistence</t>
-  </si>
-  <si>
     <t>Letten, AD; Dhami, MK; Ke, PJ; Fukami, T</t>
   </si>
   <si>
@@ -218,12 +191,6 @@
     <t>WOS:000436245000076</t>
   </si>
   <si>
-    <t>Partitioning</t>
-  </si>
-  <si>
-    <t>* used Ellner et al 2016 numerical method to quantify storage effects and relative non-linearities</t>
-  </si>
-  <si>
     <t>Zhao, L; Zhang, QG; Zhang, DY</t>
   </si>
   <si>
@@ -242,9 +209,6 @@
     <t>WOS:000382581400017</t>
   </si>
   <si>
-    <t>* tested the effect of evolution of co-existence (showcasing strength of microbial study systems)</t>
-  </si>
-  <si>
     <t>Tan, JQ; Slattery, MR; Yang, X; Jiang, L</t>
   </si>
   <si>
@@ -263,9 +227,6 @@
     <t>WOS:000381247300018</t>
   </si>
   <si>
-    <t>Calculates ND-FD but doesn‚Äôt seem to use them to explain co-existence? More about phylogenitic diversity and speciation?</t>
-  </si>
-  <si>
     <t>Narwani, A; Alexandrou, MA; Oakley, TH; Carroll, IT; Cardinale, BJ</t>
   </si>
   <si>
@@ -299,9 +260,6 @@
     <t>WOS:000247398800004</t>
   </si>
   <si>
-    <t>Lots of discussion of storage effect and relative non-linearity, but I couldn't see any application of MCT to test for these effects</t>
-  </si>
-  <si>
     <t>Descamps-Julien, B; Gonzalez, A</t>
   </si>
   <si>
@@ -320,9 +278,6 @@
     <t>WOS:000232361800026</t>
   </si>
   <si>
-    <t>Concepts from MCT I guess, but not actual methods?</t>
-  </si>
-  <si>
     <t>Jia, NN; Yang, YM; Yu, GL; Wang, YL; Qiu, PF; Li, H; Li, RH</t>
   </si>
   <si>
@@ -341,12 +296,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>INV Only</t>
-  </si>
-  <si>
-    <t>no niche/fitness difference</t>
-  </si>
-  <si>
     <t>Spaak, JW; De Laender, F</t>
   </si>
   <si>
@@ -359,9 +308,6 @@
     <t>10.1111/ele.13511</t>
   </si>
   <si>
-    <t>the empirical data is taken from Stomp et al 2004 - secondary data does not meet criterion 1</t>
-  </si>
-  <si>
     <t>Griffiths, JI; Warren, PH; Childs, DZ</t>
   </si>
   <si>
@@ -377,9 +323,6 @@
     <t>10.1111/oik.01704</t>
   </si>
   <si>
-    <t>Invasion tests only</t>
-  </si>
-  <si>
     <t>Venail, PA; Narwani, A; Fritschie, K; Alexandrou, MA; Oakley, TH; Cardinale, BJ</t>
   </si>
   <si>
@@ -395,9 +338,6 @@
     <t>10.1111/1365-2745.12271</t>
   </si>
   <si>
-    <t>Some mention of niche and fittness differences, but these weren't calculated. Study was in the context of invasions and relatedness</t>
-  </si>
-  <si>
     <t>Ontiveros, VJ; Capitan, JA; Casamayor, EO; Alonso, D</t>
   </si>
   <si>
@@ -413,9 +353,6 @@
     <t>WOS:001022964700006</t>
   </si>
   <si>
-    <t>lots of discussion of MCT and the different mechansms in intro, but not applied in methods (observational data of bacterial meta-communities). Exploring equalizing mechanisms from a colinization-extinction dynamics perspective</t>
-  </si>
-  <si>
     <t>Albert, PJ; Reuman, DC</t>
   </si>
   <si>
@@ -431,9 +368,6 @@
     <t>WOS:001101583100001</t>
   </si>
   <si>
-    <t xml:space="preserve">exploring temporal storage effect using lots of models and also empirical diatom data from Descamps-Julien and Gonzalez (2005). Excluded as the empirical data is not primary (i.e., was not generated in this study). </t>
-  </si>
-  <si>
     <t>Chang, CY; Bajic, D; Vila, JCC; Estrela, S; Sanchez, A</t>
   </si>
   <si>
@@ -452,9 +386,6 @@
     <t>WOS:001046763100034</t>
   </si>
   <si>
-    <t xml:space="preserve">pairwise competition and invasion tests only (no use of MCT) </t>
-  </si>
-  <si>
     <t>Siegel, P; Baker, KG; Low-D√©carie, E; Geider, RJ</t>
   </si>
   <si>
@@ -473,9 +404,6 @@
     <t>WOS:000954435600001</t>
   </si>
   <si>
-    <t>all about coexistence in fluctuating environments… doesn't seem to directly quantify the potenital mechanisms (e.g., temporal storage effect)</t>
-  </si>
-  <si>
     <t>Liu, X; Zhang, CZ; Yang, T; Gao, GF; Shi, Y; Chu, HY</t>
   </si>
   <si>
@@ -494,9 +422,6 @@
     <t>WOS:001069588100001</t>
   </si>
   <si>
-    <t>some discussion of niche and fitness differences but these were not quanitifed. It was more of a phylogentics-coccurrence study</t>
-  </si>
-  <si>
     <t>Schlechter, RO; Kear, EJ; Bernach, M; Remus, DM; Remus-Emsermann, MNP</t>
   </si>
   <si>
@@ -512,9 +437,6 @@
     <t>WOS:001019919800001</t>
   </si>
   <si>
-    <t>doesn't quantify niche AND fitness differences - just "competition score" (which would be fitness differences only) based on Chesson's framework… Not sure really</t>
-  </si>
-  <si>
     <t>Choi, S; Yang, JW; Kim, JE; Jeon, H; Shin, S; Wui, D; Kim, LS; Kim, BJ; Son, H; Min, K</t>
   </si>
   <si>
@@ -533,9 +455,6 @@
     <t>WOS:001064083600001</t>
   </si>
   <si>
-    <t>mentions MCT but doesn't use it</t>
-  </si>
-  <si>
     <t>Zuo, J; Liu, LM; Xiao, P; Xu, ZJ; Wilkinson, DM; Grossart, HP; Chen, HH; Yang, J</t>
   </si>
   <si>
@@ -554,9 +473,6 @@
     <t>WOS:001069980400001</t>
   </si>
   <si>
-    <t>mentions FD and ND but does not quantify them</t>
-  </si>
-  <si>
     <t>Kuhn, T; Mamin, M; Bindschedler, S; Bshary, R; Estoppey, A; Gonzalez, D; Palmieri, F; Junier, P; Richter, XYL</t>
   </si>
   <si>
@@ -575,9 +491,6 @@
     <t>WOS:000894035200003</t>
   </si>
   <si>
-    <t>no mention or use of MCT</t>
-  </si>
-  <si>
     <t>Zhou, ZY; Xiao, M; Wang, SL; Wang, XY; Li, W; Chen, Y; Yuan, ZL; Guo, EH</t>
   </si>
   <si>
@@ -596,9 +509,6 @@
     <t>WOS:000817359600001</t>
   </si>
   <si>
-    <t>all about "temporal partitioning hypothesis" - not sure what this is? Doesn't seem to engage with MCT?</t>
-  </si>
-  <si>
     <t>Zhang, N; Nunan, N; Hirsch, PR; Sun, B; Zhou, JZ; Liang, YT</t>
   </si>
   <si>
@@ -617,9 +527,6 @@
     <t>WOS:000689631900001</t>
   </si>
   <si>
-    <t>review paper</t>
-  </si>
-  <si>
     <t>Wisnoski, NI; Lennon, JT</t>
   </si>
   <si>
@@ -635,9 +542,6 @@
     <t>WOS:000678531800001</t>
   </si>
   <si>
-    <t>observational data but it seems to be collected in part at least for this work? Exploring negative frequency dependence as a mechanism for coexistence</t>
-  </si>
-  <si>
     <t>Letten, AD; Hall, AR; Levine, JM</t>
   </si>
   <si>
@@ -656,9 +560,6 @@
     <t>WOS:000613622000002</t>
   </si>
   <si>
-    <t>no empirical data</t>
-  </si>
-  <si>
     <t>Zufiaurre, A; Felip, M; Gim√©nez-Grau, P; Pla-Rab√®s, S; Camarero, L; Catalan, J</t>
   </si>
   <si>
@@ -674,9 +575,6 @@
     <t>WOS:000612358100001</t>
   </si>
   <si>
-    <t>used MCT (ND and FD) to explore effects of nutrients on the coexistence of different protists from a lake</t>
-  </si>
-  <si>
     <t>Effects of pigment richness and size variation on coexistence, richness and function in light-limited phytoplankton</t>
   </si>
   <si>
@@ -689,9 +587,6 @@
     <t>WOS:000634536300001</t>
   </si>
   <si>
-    <t>used MCT to study a classic light-phytoplankton model and compared it's predictions to some secondary data</t>
-  </si>
-  <si>
     <t>Abreu, CI; Woltz, VAL; Friedman, J; Gore, J</t>
   </si>
   <si>
@@ -1097,9 +992,6 @@
     <t>Taxanomic group</t>
   </si>
   <si>
-    <t>Rough categorization of the way MCT was applied (for screeners use for now)</t>
-  </si>
-  <si>
     <t>Whether the paper was in the Web of Science search used (yes or no)</t>
   </si>
   <si>
@@ -1109,9 +1001,6 @@
     <t>Whether the paper was used to initialize/train the machine learning model for asreview screening (yes or no)</t>
   </si>
   <si>
-    <t xml:space="preserve">Note to screeners to help with decision making </t>
-  </si>
-  <si>
     <t xml:space="preserve">Whether the paper was included following full text screening (yes or no) </t>
   </si>
   <si>
@@ -1121,9 +1010,6 @@
     <t>Whether the paper was found from previous syntheses (yes or no)</t>
   </si>
   <si>
-    <t>Note to collaborators that this paper would be worth discussing (e.g., not relevant but borrowed concepts from MCT)</t>
-  </si>
-  <si>
     <t>Order in which the papers were found during abstract screening</t>
   </si>
   <si>
@@ -1145,72 +1031,6 @@
     <t>Authors of paper</t>
   </si>
   <si>
-    <t>explores coexistence in fluctuating environments but not using MCT framework</t>
-  </si>
-  <si>
-    <t>secondary data (large biomonitoring program) analysed with MAR to estiamte competition coefficients to study coexistence - but not using core MCT framework</t>
-  </si>
-  <si>
-    <t>resource competition theory instead of MCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secondary data analysed without MCT but discussed using concepts from MCT </t>
-  </si>
-  <si>
-    <t>competition experiments and relative fitness differences but no niche differences or engagement with MCT</t>
-  </si>
-  <si>
-    <t>talks about lotery effects but doesn't use MCT</t>
-  </si>
-  <si>
-    <t>uses resource competition theory rather than MCT to explore coexistence</t>
-  </si>
-  <si>
-    <t>analyses the data from the perspective of resource competition and focuses on niche differentiation (discusses how findings fit in with MCT)</t>
-  </si>
-  <si>
-    <t>explores coexistence but not from MCT perspective</t>
-  </si>
-  <si>
-    <t>explores an evolutionary mechanism (nonlinear frequency dependent selection) for coexistence of bacteria</t>
-  </si>
-  <si>
-    <t>niche and fitness differences quanitfied using Carrol method and used to study adaptive radiation/colinization history for bacterial communities</t>
-  </si>
-  <si>
-    <t>niche and fitness differences quanitfied using Carrol method and used to study coexistence in the context of MCT and spatial storage effects for bacterial metacommunities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">competition experiments, fit to LV for competition coefficients but no niche and fitness differences directly measured here - instead relative density and gene expression/phylogenietic relatedness were the topic of interest. Lots of discussion of MCT but they do explicitly say that they didn't directly measure ND and FD in this study. </t>
-  </si>
-  <si>
-    <t>modelling study that doesn’t use MCT directly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modelling study that uses secondary data to test models and doesn’t employ MCT </t>
-  </si>
-  <si>
-    <t>pairwise competition and interactions quantified by fitting to LV models - discussion of concepts from MCT, but MCT itself not applied</t>
-  </si>
-  <si>
-    <t>in the realms of MCT, but more about temporal niches and adaptive radiations</t>
-  </si>
-  <si>
-    <t>discusses some MCT concepts, but mostly from the perspective of resoruce competition theory</t>
-  </si>
-  <si>
-    <t>secondary data and niche and fitness differences weren't both quantified</t>
-  </si>
-  <si>
-    <t>lots of discussion of MCT, but niche and fitness differences weren't directly quantified</t>
-  </si>
-  <si>
-    <t>empirical test of general ideas from early coexistence theory, but no niche/fitness differences or quantifying specific mechanisms</t>
-  </si>
-  <si>
-    <t>empirical test of ideas about fluctuating envrionments and coexistence with reference to early Chesson work - but not formal MCT</t>
-  </si>
-  <si>
     <t>WOS:000555112000008</t>
   </si>
   <si>
@@ -1223,7 +1043,49 @@
     <t>WOS:000340681300019</t>
   </si>
   <si>
-    <t>MCT was refered to but not actually employed</t>
+    <t>Asreview</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>ASReview Found</t>
+  </si>
+  <si>
+    <t>statistical analyses only</t>
+  </si>
+  <si>
+    <t>resource competition theory</t>
+  </si>
+  <si>
+    <t>metacommunity theory</t>
+  </si>
+  <si>
+    <t>competition coefficients</t>
+  </si>
+  <si>
+    <t>negative frequency dependence</t>
+  </si>
+  <si>
+    <t>invasion analysis</t>
+  </si>
+  <si>
+    <t>Alternative Analysis</t>
+  </si>
+  <si>
+    <t>For the papers that were excluded for not applying MCT but that were in microbial systems and were primary studies, what analytical framework did they use?</t>
+  </si>
+  <si>
+    <t>invasion analysis, lotka-voltera</t>
+  </si>
+  <si>
+    <t>lotka-voltera</t>
+  </si>
+  <si>
+    <t>lotka-voltera, resource competition theory</t>
   </si>
 </sst>
 </file>
@@ -1714,9 +1576,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2092,15 +1957,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T55"/>
+  <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="22" max="22" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2147,3044 +2016,2909 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
       </c>
       <c r="E2">
         <v>2022</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O2">
+        <v>151</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D3" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2">
-        <v>151</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
       </c>
       <c r="E3">
         <v>2020</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" t="s">
-        <v>105</v>
-      </c>
-      <c r="P3">
+        <v>90</v>
+      </c>
+      <c r="O3">
         <v>327</v>
       </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
       <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>2019</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="O4" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="P4" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
       </c>
       <c r="E5">
         <v>2019</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5">
+        <v>90</v>
+      </c>
+      <c r="O5">
         <v>8</v>
       </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
       <c r="Q5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" t="s">
-        <v>26</v>
-      </c>
-      <c r="S5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>2019</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P6">
+        <v>90</v>
+      </c>
+      <c r="O6">
         <v>10</v>
       </c>
+      <c r="P6" t="s">
+        <v>21</v>
+      </c>
       <c r="Q6" t="s">
-        <v>59</v>
-      </c>
-      <c r="R6" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E7">
         <v>2018</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="M7" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" t="s">
-        <v>26</v>
-      </c>
-      <c r="S7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E8">
         <v>2016</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s">
-        <v>105</v>
-      </c>
-      <c r="P8">
+        <v>90</v>
+      </c>
+      <c r="O8">
         <v>18</v>
       </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
       <c r="Q8" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8" t="s">
-        <v>26</v>
-      </c>
-      <c r="S8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E9">
         <v>2016</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" t="s">
-        <v>105</v>
-      </c>
-      <c r="P9">
+        <v>90</v>
+      </c>
+      <c r="O9">
         <v>19</v>
       </c>
+      <c r="P9" t="s">
+        <v>21</v>
+      </c>
       <c r="Q9" t="s">
-        <v>80</v>
-      </c>
-      <c r="R9" t="s">
-        <v>26</v>
-      </c>
-      <c r="S9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E10">
         <v>2013</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" t="s">
         <v>37</v>
       </c>
-      <c r="M10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" t="s">
-        <v>26</v>
-      </c>
       <c r="P10" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="Q10" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" t="s">
-        <v>26</v>
-      </c>
-      <c r="S10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E11">
         <v>2007</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K11" t="s">
-        <v>105</v>
-      </c>
-      <c r="L11" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" t="s">
-        <v>105</v>
-      </c>
-      <c r="P11">
+        <v>90</v>
+      </c>
+      <c r="O11">
         <v>92</v>
       </c>
+      <c r="P11" t="s">
+        <v>21</v>
+      </c>
       <c r="Q11" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="R11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S11" t="s">
-        <v>26</v>
-      </c>
-      <c r="T11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E12">
         <v>2005</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" t="s">
-        <v>105</v>
-      </c>
-      <c r="P12">
+        <v>90</v>
+      </c>
+      <c r="O12">
         <v>72</v>
       </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
       <c r="Q12" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="R12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S12" t="s">
-        <v>26</v>
-      </c>
-      <c r="T12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <v>2020</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>396</v>
+        <v>336</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K13" t="s">
-        <v>105</v>
-      </c>
-      <c r="L13" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="M13" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O13" t="s">
-        <v>105</v>
+        <v>317</v>
       </c>
       <c r="P13" t="s">
-        <v>352</v>
+        <v>90</v>
       </c>
       <c r="Q13" t="s">
-        <v>107</v>
-      </c>
-      <c r="R13" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="S13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="E14">
         <v>2020</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>397</v>
+        <v>337</v>
       </c>
       <c r="H14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K14" t="s">
-        <v>105</v>
-      </c>
-      <c r="L14" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="M14" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="N14" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="O14" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="P14" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="Q14" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="R14" t="s">
-        <v>105</v>
-      </c>
-      <c r="S14" t="s">
-        <v>26</v>
-      </c>
-      <c r="T14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E15">
         <v>2015</v>
       </c>
       <c r="F15" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="G15" t="s">
-        <v>398</v>
+        <v>338</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K15" t="s">
-        <v>105</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="N15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="O15" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="P15" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="Q15" t="s">
-        <v>118</v>
-      </c>
-      <c r="R15" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="S15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E16">
         <v>2014</v>
       </c>
       <c r="F16" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G16" t="s">
-        <v>399</v>
+        <v>339</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K16" t="s">
+        <v>90</v>
+      </c>
+      <c r="M16" t="s">
+        <v>90</v>
+      </c>
+      <c r="N16" t="s">
+        <v>90</v>
+      </c>
+      <c r="O16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>105</v>
       </c>
-      <c r="K16" t="s">
-        <v>105</v>
-      </c>
-      <c r="L16" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="B17" t="s">
         <v>106</v>
       </c>
-      <c r="N16" t="s">
-        <v>105</v>
-      </c>
-      <c r="O16" t="s">
-        <v>105</v>
-      </c>
-      <c r="P16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>124</v>
-      </c>
-      <c r="R16" t="s">
-        <v>105</v>
-      </c>
-      <c r="S16" t="s">
-        <v>26</v>
-      </c>
-      <c r="T16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
-      </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="E17">
         <v>2023</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K17" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M17" t="s">
+        <v>21</v>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O17" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P17" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q17" t="s">
-        <v>130</v>
-      </c>
-      <c r="R17" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="E18">
         <v>2023</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M18" t="s">
+        <v>21</v>
       </c>
       <c r="N18" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O18" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P18" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q18" t="s">
-        <v>136</v>
-      </c>
-      <c r="R18" t="s">
-        <v>26</v>
-      </c>
-      <c r="S18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E19">
         <v>2023</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J19" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K19" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M19" t="s">
+        <v>21</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P19" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q19" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="R19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S19" t="s">
-        <v>105</v>
-      </c>
-      <c r="T19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="E20">
         <v>2023</v>
       </c>
       <c r="F20" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="H20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J20" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K20" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M20" t="s">
+        <v>21</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O20" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P20" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q20" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="R20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S20" t="s">
-        <v>105</v>
-      </c>
-      <c r="T20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="E21">
         <v>2023</v>
       </c>
       <c r="F21" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J21" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M21" t="s">
+        <v>21</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O21" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P21" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q21" t="s">
-        <v>157</v>
-      </c>
-      <c r="R21" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="E22">
         <v>2023</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="G22" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="H22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J22" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K22" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M22" t="s">
+        <v>21</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O22" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P22" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q22" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="R22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S22" t="s">
-        <v>105</v>
-      </c>
-      <c r="T22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="E23">
         <v>2023</v>
       </c>
       <c r="F23" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="G23" t="s">
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="H23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J23" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K23" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M23" t="s">
+        <v>21</v>
       </c>
       <c r="N23" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O23" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P23" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q23" t="s">
-        <v>170</v>
-      </c>
-      <c r="R23" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="E24">
         <v>2023</v>
       </c>
       <c r="F24" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="G24" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="H24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K24" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M24" t="s">
+        <v>21</v>
       </c>
       <c r="N24" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O24" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P24" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q24" t="s">
-        <v>177</v>
-      </c>
-      <c r="R24" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="E25">
         <v>2022</v>
       </c>
       <c r="F25" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="G25" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="H25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J25" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K25" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M25" t="s">
+        <v>21</v>
       </c>
       <c r="N25" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O25" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P25" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q25" t="s">
-        <v>184</v>
-      </c>
-      <c r="R25" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="D26" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="E26">
         <v>2022</v>
       </c>
       <c r="F26" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="H26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K26" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M26" t="s">
+        <v>21</v>
       </c>
       <c r="N26" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O26" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P26" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q26" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="R26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S26" t="s">
-        <v>105</v>
-      </c>
-      <c r="T26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="D27" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="E27">
         <v>2021</v>
       </c>
       <c r="F27" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="G27" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="H27" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K27" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M27" t="s">
+        <v>21</v>
       </c>
       <c r="N27" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O27" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P27" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q27" t="s">
-        <v>198</v>
-      </c>
-      <c r="R27" t="s">
-        <v>26</v>
-      </c>
-      <c r="S27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="E28">
         <v>2021</v>
       </c>
       <c r="F28" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="G28" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="H28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J28" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K28" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M28" t="s">
+        <v>21</v>
       </c>
       <c r="N28" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O28" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P28" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q28" t="s">
-        <v>204</v>
+        <v>90</v>
       </c>
       <c r="R28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S28" t="s">
-        <v>105</v>
-      </c>
-      <c r="T28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="C29" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="E29">
         <v>2021</v>
       </c>
       <c r="F29" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="G29" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="H29" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M29" t="s">
+        <v>21</v>
       </c>
       <c r="N29" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O29" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P29" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q29" t="s">
-        <v>211</v>
-      </c>
-      <c r="R29" t="s">
-        <v>26</v>
-      </c>
-      <c r="S29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="E30">
         <v>2021</v>
       </c>
       <c r="F30" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="G30" t="s">
-        <v>216</v>
+        <v>183</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N30" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O30" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P30" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q30" t="s">
-        <v>217</v>
-      </c>
-      <c r="R30" t="s">
-        <v>26</v>
-      </c>
-      <c r="S30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="E31">
         <v>2021</v>
       </c>
       <c r="F31" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="G31" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="H31" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I31" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J31" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K31" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M31" t="s">
+        <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O31" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P31" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q31" t="s">
-        <v>222</v>
-      </c>
-      <c r="R31" t="s">
-        <v>26</v>
-      </c>
-      <c r="S31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="B32" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="C32" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="D32" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="E32">
         <v>2020</v>
       </c>
       <c r="F32" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="G32" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="H32" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I32" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K32" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M32" t="s">
+        <v>21</v>
       </c>
       <c r="N32" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O32" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P32" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q32" t="s">
-        <v>374</v>
-      </c>
-      <c r="R32" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+      <c r="V32" s="2"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="E33">
         <v>2020</v>
       </c>
       <c r="F33" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="G33" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
       <c r="H33" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I33" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J33" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K33" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M33" t="s">
+        <v>21</v>
       </c>
       <c r="N33" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O33" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P33" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q33" t="s">
-        <v>375</v>
-      </c>
-      <c r="R33" t="s">
-        <v>26</v>
-      </c>
-      <c r="S33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="B34" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
       <c r="D34" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
       <c r="E34">
         <v>2020</v>
       </c>
       <c r="F34" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
       <c r="G34" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I34" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K34" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M34" t="s">
+        <v>21</v>
       </c>
       <c r="N34" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O34" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P34" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q34" t="s">
-        <v>376</v>
-      </c>
-      <c r="R34" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+      <c r="V34" s="2"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="E35">
         <v>2020</v>
       </c>
       <c r="F35" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="G35" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="H35" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K35" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M35" t="s">
+        <v>21</v>
       </c>
       <c r="N35" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O35" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P35" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q35" t="s">
-        <v>377</v>
+        <v>90</v>
       </c>
       <c r="R35" t="s">
-        <v>26</v>
-      </c>
-      <c r="S35" t="s">
-        <v>105</v>
-      </c>
-      <c r="T35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
       <c r="B36" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="D36" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="E36">
         <v>2020</v>
       </c>
       <c r="F36" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="G36" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="H36" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I36" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K36" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M36" t="s">
+        <v>21</v>
       </c>
       <c r="N36" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O36" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P36" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q36" t="s">
-        <v>378</v>
-      </c>
-      <c r="R36" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="D37" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="E37">
         <v>2019</v>
       </c>
       <c r="F37" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="G37" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="H37" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I37" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J37" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K37" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M37" t="s">
+        <v>21</v>
       </c>
       <c r="N37" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O37" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P37" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q37" t="s">
-        <v>379</v>
-      </c>
-      <c r="R37" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="V37" s="2"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="B38" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="C38" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="D38" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="E38">
         <v>2019</v>
       </c>
       <c r="F38" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="G38" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="H38" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K38" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M38" t="s">
+        <v>21</v>
       </c>
       <c r="N38" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O38" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P38" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q38" t="s">
-        <v>211</v>
-      </c>
-      <c r="R38" t="s">
-        <v>26</v>
-      </c>
-      <c r="S38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="B39" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="E39">
         <v>2019</v>
       </c>
       <c r="F39" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
       <c r="G39" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
       <c r="H39" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I39" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J39" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K39" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M39" t="s">
+        <v>21</v>
       </c>
       <c r="N39" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O39" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P39" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q39" t="s">
-        <v>380</v>
-      </c>
-      <c r="R39" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S39" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
       <c r="E40">
         <v>2019</v>
       </c>
       <c r="F40" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="G40" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="H40" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I40" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J40" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K40" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
       </c>
       <c r="N40" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O40" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P40" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q40" t="s">
-        <v>381</v>
-      </c>
-      <c r="R40" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="B41" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D41" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="E41">
         <v>2019</v>
       </c>
       <c r="F41" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="G41" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
       <c r="H41" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I41" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J41" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K41" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M41" t="s">
+        <v>21</v>
       </c>
       <c r="N41" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O41" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P41" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q41" t="s">
-        <v>382</v>
-      </c>
-      <c r="R41" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="B42" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="E42">
         <v>2019</v>
       </c>
       <c r="F42" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="G42" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
       <c r="H42" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I42" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J42" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K42" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M42" t="s">
+        <v>21</v>
       </c>
       <c r="N42" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O42" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P42" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q42" t="s">
-        <v>383</v>
+        <v>90</v>
       </c>
       <c r="R42" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S42" t="s">
-        <v>105</v>
-      </c>
-      <c r="T42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="B43" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="C43" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="D43" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="E43">
         <v>2017</v>
       </c>
       <c r="F43" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="G43" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
       <c r="H43" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I43" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J43" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K43" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L43" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M43" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N43" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O43" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P43" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q43" t="s">
-        <v>384</v>
-      </c>
-      <c r="R43" t="s">
-        <v>26</v>
-      </c>
-      <c r="S43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="B44" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="E44">
         <v>2017</v>
       </c>
       <c r="F44" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="G44" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
       <c r="H44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K44" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L44" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M44" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N44" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O44" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P44" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q44" t="s">
-        <v>385</v>
-      </c>
-      <c r="R44" t="s">
-        <v>26</v>
-      </c>
-      <c r="S44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="B45" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="C45" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="E45">
         <v>2017</v>
       </c>
       <c r="F45" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="G45" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="H45" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I45" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J45" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K45" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M45" t="s">
+        <v>21</v>
       </c>
       <c r="N45" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O45" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P45" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q45" t="s">
-        <v>386</v>
+        <v>90</v>
       </c>
       <c r="R45" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S45" t="s">
-        <v>105</v>
-      </c>
-      <c r="T45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="C46" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="D46" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="E46">
         <v>2016</v>
       </c>
       <c r="F46" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="G46" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="H46" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I46" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J46" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K46" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M46" t="s">
+        <v>21</v>
       </c>
       <c r="N46" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O46" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P46" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q46" t="s">
-        <v>387</v>
-      </c>
-      <c r="R46" t="s">
-        <v>26</v>
-      </c>
-      <c r="S46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="B47" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="C47" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="D47" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
       <c r="E47">
         <v>2015</v>
       </c>
       <c r="F47" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
       <c r="G47" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="H47" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I47" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J47" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K47" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M47" t="s">
+        <v>21</v>
       </c>
       <c r="N47" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O47" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P47" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q47" t="s">
-        <v>388</v>
-      </c>
-      <c r="R47" t="s">
-        <v>26</v>
-      </c>
-      <c r="S47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
       <c r="B48" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
       <c r="E48">
         <v>2015</v>
       </c>
       <c r="F48" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="G48" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="H48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J48" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K48" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M48" t="s">
+        <v>21</v>
       </c>
       <c r="N48" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O48" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P48" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q48" t="s">
-        <v>389</v>
+        <v>90</v>
       </c>
       <c r="R48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="S48" t="s">
-        <v>105</v>
-      </c>
-      <c r="T48" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
       <c r="B49" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="C49" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
       <c r="D49" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="E49">
         <v>2013</v>
       </c>
       <c r="F49" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="G49" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
       <c r="H49" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I49" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J49" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K49" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M49" t="s">
+        <v>21</v>
       </c>
       <c r="N49" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O49" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P49" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q49" t="s">
-        <v>390</v>
-      </c>
-      <c r="R49" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="B50" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>322</v>
+        <v>287</v>
       </c>
       <c r="E50">
         <v>2011</v>
       </c>
       <c r="F50" t="s">
-        <v>323</v>
+        <v>288</v>
       </c>
       <c r="G50" t="s">
+        <v>289</v>
+      </c>
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" t="s">
+        <v>90</v>
+      </c>
+      <c r="K50" t="s">
+        <v>90</v>
+      </c>
+      <c r="M50" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" t="s">
+        <v>90</v>
+      </c>
+      <c r="O50" t="s">
         <v>324</v>
       </c>
-      <c r="H50" t="s">
-        <v>26</v>
-      </c>
-      <c r="I50" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" t="s">
-        <v>105</v>
-      </c>
-      <c r="K50" t="s">
-        <v>105</v>
-      </c>
-      <c r="N50" t="s">
-        <v>26</v>
-      </c>
-      <c r="O50" t="s">
-        <v>105</v>
-      </c>
       <c r="P50" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q50" t="s">
-        <v>391</v>
-      </c>
-      <c r="R50" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>327</v>
+        <v>292</v>
       </c>
       <c r="E51">
         <v>2010</v>
       </c>
       <c r="F51" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
       <c r="G51" t="s">
-        <v>329</v>
+        <v>294</v>
       </c>
       <c r="H51" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I51" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J51" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K51" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M51" t="s">
+        <v>21</v>
       </c>
       <c r="N51" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O51" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P51" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q51" t="s">
-        <v>392</v>
-      </c>
-      <c r="R51" t="s">
-        <v>26</v>
-      </c>
-      <c r="S51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="B52" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D52" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="E52">
         <v>2009</v>
       </c>
       <c r="F52" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="G52" t="s">
-        <v>334</v>
+        <v>299</v>
       </c>
       <c r="H52" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I52" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J52" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K52" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M52" t="s">
+        <v>21</v>
       </c>
       <c r="N52" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O52" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P52" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q52" t="s">
-        <v>393</v>
-      </c>
-      <c r="R52" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
       <c r="B53" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="E53">
         <v>2009</v>
       </c>
       <c r="F53" t="s">
-        <v>338</v>
+        <v>303</v>
       </c>
       <c r="G53" t="s">
-        <v>339</v>
+        <v>304</v>
       </c>
       <c r="H53" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I53" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J53" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K53" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M53" t="s">
+        <v>21</v>
       </c>
       <c r="N53" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O53" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P53" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q53" t="s">
-        <v>400</v>
-      </c>
-      <c r="R53" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S53" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="B54" t="s">
-        <v>341</v>
+        <v>306</v>
       </c>
       <c r="C54" t="s">
-        <v>342</v>
+        <v>307</v>
       </c>
       <c r="D54" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
       <c r="E54">
         <v>2006</v>
       </c>
       <c r="F54" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="G54" t="s">
+        <v>310</v>
+      </c>
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" t="s">
+        <v>90</v>
+      </c>
+      <c r="K54" t="s">
+        <v>90</v>
+      </c>
+      <c r="M54" t="s">
+        <v>21</v>
+      </c>
+      <c r="N54" t="s">
+        <v>90</v>
+      </c>
+      <c r="O54" t="s">
+        <v>324</v>
+      </c>
+      <c r="P54" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>90</v>
+      </c>
+      <c r="R54" t="s">
+        <v>21</v>
+      </c>
+      <c r="S54" t="s">
         <v>345</v>
       </c>
-      <c r="H54" t="s">
-        <v>26</v>
-      </c>
-      <c r="I54" t="s">
-        <v>26</v>
-      </c>
-      <c r="J54" t="s">
-        <v>105</v>
-      </c>
-      <c r="K54" t="s">
-        <v>105</v>
-      </c>
-      <c r="N54" t="s">
-        <v>26</v>
-      </c>
-      <c r="O54" t="s">
-        <v>105</v>
-      </c>
-      <c r="P54" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>394</v>
-      </c>
-      <c r="R54" t="s">
-        <v>26</v>
-      </c>
-      <c r="S54" t="s">
-        <v>105</v>
-      </c>
-      <c r="T54" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>346</v>
+        <v>311</v>
       </c>
       <c r="B55" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
       <c r="C55" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="D55" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
       <c r="E55">
         <v>2006</v>
       </c>
       <c r="F55" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="G55" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="H55" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I55" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J55" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="K55" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="M55" t="s">
+        <v>21</v>
       </c>
       <c r="N55" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O55" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="P55" t="s">
-        <v>360</v>
+        <v>21</v>
       </c>
       <c r="Q55" t="s">
-        <v>395</v>
-      </c>
-      <c r="R55" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="S55" t="s">
-        <v>105</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5197,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5205,7 +4939,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5213,7 +4947,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -5221,7 +4955,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5229,7 +4963,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5237,7 +4971,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -5245,7 +4979,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -5253,7 +4987,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5261,7 +4995,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5269,7 +5003,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5277,7 +5011,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5285,7 +5019,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>357</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5293,7 +5027,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5301,55 +5035,39 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
-        <v>361</v>
+        <v>329</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>340</v>
       </c>
       <c r="B16" t="s">
-        <v>367</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>341</v>
       </c>
       <c r="B17" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="B18" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>